<commit_message>
Fixes #2861 .  This does not change any C++ code.  Documentation is updated, mostly concerning mass lumping.  Some more tests utilising mass lumping are added
</commit_message>
<xml_diff>
--- a/modules/richards/doc/tests/data/rsc.xlsx
+++ b/modules/richards/doc/tests/data/rsc.xlsx
@@ -9,13 +9,15 @@
   <sheets>
     <sheet name="comparison" sheetId="4" r:id="rId1"/>
     <sheet name="rsc01" sheetId="1" r:id="rId2"/>
-    <sheet name="rsc02" sheetId="5" r:id="rId3"/>
-    <sheet name="rsc_analytic" sheetId="2" r:id="rId4"/>
+    <sheet name="rsc_lumped_01" sheetId="6" r:id="rId3"/>
+    <sheet name="rsc02" sheetId="5" r:id="rId4"/>
+    <sheet name="rsc_analytic" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="rsc01_" localSheetId="2">rsc_lumped_01!$C$3:$L$54</definedName>
     <definedName name="rsc01_" localSheetId="1">'rsc01'!$C$3:$L$54</definedName>
-    <definedName name="rsc01_analytic" localSheetId="3">rsc_analytic!$C$3:$D$33</definedName>
-    <definedName name="rsc02_" localSheetId="2">'rsc02'!$C$3:$L$54</definedName>
+    <definedName name="rsc01_analytic" localSheetId="4">rsc_analytic!$C$3:$D$33</definedName>
+    <definedName name="rsc02_" localSheetId="3">'rsc02'!$C$3:$L$54</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -24,7 +26,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="rsc01" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="L:\moose\project2\trunk\elk\doc\richards\tests\data\rsc01.csv" comma="1">
+    <textPr codePage="850" sourceFile="L:\moose\projects_andy\moose\modules\richards\doc\tests\data\rsc01.csv" comma="1">
       <textFields count="10">
         <textField/>
         <textField/>
@@ -47,7 +49,23 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="rsc02" type="6" refreshedVersion="3" background="1" saveData="1">
+  <connection id="3" name="rsc011" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="L:\moose\projects_andy\moose\modules\richards\doc\tests\data\rsc_lumped_01.csv" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="rsc02" type="6" refreshedVersion="3" background="1" saveData="1">
     <textPr codePage="850" sourceFile="L:\moose\project2\trunk\elk\doc\richards\tests\data\rsc02.csv" comma="1">
       <textFields count="10">
         <textField/>
@@ -67,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>pwater</t>
   </si>
@@ -1071,11 +1089,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="156001792"/>
-        <c:axId val="156003328"/>
+        <c:axId val="137898240"/>
+        <c:axId val="137929088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="156001792"/>
+        <c:axId val="137898240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1098,12 +1116,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156003328"/>
+        <c:crossAx val="137929088"/>
         <c:crossesAt val="7"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="156003328"/>
+        <c:axId val="137929088"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="7"/>
@@ -1135,7 +1153,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156001792"/>
+        <c:crossAx val="137898240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1154,7 +1172,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1193,10 +1211,14 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rsc02" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rsc01" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rsc02" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rsc01_analytic" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -3175,6 +3197,1694 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:L54"/>
   <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:12">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12">
+      <c r="C4">
+        <v>3.4397999999999998E-3</v>
+      </c>
+      <c r="D4">
+        <v>0.99656</v>
+      </c>
+      <c r="E4">
+        <v>171.09</v>
+      </c>
+      <c r="F4">
+        <v>166.07</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12">
+      <c r="C5">
+        <v>1.5810000000000001E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.98419000000000001</v>
+      </c>
+      <c r="E5">
+        <v>170.62</v>
+      </c>
+      <c r="F5">
+        <v>164.05</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0.2</v>
+      </c>
+      <c r="J5">
+        <v>0.2</v>
+      </c>
+      <c r="K5">
+        <v>1E-3</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12">
+      <c r="C6">
+        <v>4.3776000000000002E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.95621999999999996</v>
+      </c>
+      <c r="E6">
+        <v>169.64</v>
+      </c>
+      <c r="F6">
+        <v>162.01</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0.40000999999999998</v>
+      </c>
+      <c r="J6">
+        <v>0.4</v>
+      </c>
+      <c r="K6">
+        <v>2E-3</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12">
+      <c r="C7">
+        <v>9.1359999999999997E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.90864</v>
+      </c>
+      <c r="E7">
+        <v>168.37</v>
+      </c>
+      <c r="F7">
+        <v>159.91999999999999</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0.60001000000000004</v>
+      </c>
+      <c r="J7">
+        <v>0.6</v>
+      </c>
+      <c r="K7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12">
+      <c r="C8">
+        <v>0.15647</v>
+      </c>
+      <c r="D8">
+        <v>0.84353</v>
+      </c>
+      <c r="E8">
+        <v>166.87</v>
+      </c>
+      <c r="F8">
+        <v>157.77000000000001</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0.80001</v>
+      </c>
+      <c r="J8">
+        <v>0.8</v>
+      </c>
+      <c r="K8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12">
+      <c r="C9">
+        <v>0.23225000000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.76775000000000004</v>
+      </c>
+      <c r="E9">
+        <v>165.16</v>
+      </c>
+      <c r="F9">
+        <v>155.52000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12">
+      <c r="C10">
+        <v>0.31109999999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.68889999999999996</v>
+      </c>
+      <c r="E10">
+        <v>163.28</v>
+      </c>
+      <c r="F10">
+        <v>153.18</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1.2</v>
+      </c>
+      <c r="J10">
+        <v>1.2</v>
+      </c>
+      <c r="K10">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12">
+      <c r="C11">
+        <v>0.38736999999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.61263000000000001</v>
+      </c>
+      <c r="E11">
+        <v>161.22999999999999</v>
+      </c>
+      <c r="F11">
+        <v>150.72</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1.4</v>
+      </c>
+      <c r="J11">
+        <v>1.4</v>
+      </c>
+      <c r="K11">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12">
+      <c r="C12">
+        <v>0.45795999999999998</v>
+      </c>
+      <c r="D12">
+        <v>0.54203999999999997</v>
+      </c>
+      <c r="E12">
+        <v>159.03</v>
+      </c>
+      <c r="F12">
+        <v>148.15</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1.6</v>
+      </c>
+      <c r="J12">
+        <v>1.6</v>
+      </c>
+      <c r="K12">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12">
+      <c r="C13">
+        <v>0.52164999999999995</v>
+      </c>
+      <c r="D13">
+        <v>0.47835</v>
+      </c>
+      <c r="E13">
+        <v>156.68</v>
+      </c>
+      <c r="F13">
+        <v>145.46</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1.8</v>
+      </c>
+      <c r="J13">
+        <v>1.8</v>
+      </c>
+      <c r="K13">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12">
+      <c r="C14">
+        <v>0.57830000000000004</v>
+      </c>
+      <c r="D14">
+        <v>0.42170000000000002</v>
+      </c>
+      <c r="E14">
+        <v>154.19999999999999</v>
+      </c>
+      <c r="F14">
+        <v>142.66999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>0.01</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12">
+      <c r="C15">
+        <v>0.62831999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.37168000000000001</v>
+      </c>
+      <c r="E15">
+        <v>151.59</v>
+      </c>
+      <c r="F15">
+        <v>139.76</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K15">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12">
+      <c r="C16">
+        <v>0.67232000000000003</v>
+      </c>
+      <c r="D16">
+        <v>0.32768000000000003</v>
+      </c>
+      <c r="E16">
+        <v>148.87</v>
+      </c>
+      <c r="F16">
+        <v>136.75</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>2.4</v>
+      </c>
+      <c r="J16">
+        <v>2.4</v>
+      </c>
+      <c r="K16">
+        <v>1.2E-2</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12">
+      <c r="C17">
+        <v>0.71094999999999997</v>
+      </c>
+      <c r="D17">
+        <v>0.28904999999999997</v>
+      </c>
+      <c r="E17">
+        <v>146.03</v>
+      </c>
+      <c r="F17">
+        <v>133.63999999999999</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>2.6</v>
+      </c>
+      <c r="J17">
+        <v>2.6</v>
+      </c>
+      <c r="K17">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12">
+      <c r="C18">
+        <v>0.74478</v>
+      </c>
+      <c r="D18">
+        <v>0.25522</v>
+      </c>
+      <c r="E18">
+        <v>143.09</v>
+      </c>
+      <c r="F18">
+        <v>130.43</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>2.8</v>
+      </c>
+      <c r="J18">
+        <v>2.8</v>
+      </c>
+      <c r="K18">
+        <v>1.4E-2</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12">
+      <c r="C19">
+        <v>0.77436000000000005</v>
+      </c>
+      <c r="D19">
+        <v>0.22564000000000001</v>
+      </c>
+      <c r="E19">
+        <v>140.06</v>
+      </c>
+      <c r="F19">
+        <v>127.13</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12">
+      <c r="C20">
+        <v>0.80010999999999999</v>
+      </c>
+      <c r="D20">
+        <v>0.19989000000000001</v>
+      </c>
+      <c r="E20">
+        <v>136.94</v>
+      </c>
+      <c r="F20">
+        <v>123.76</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>3.2</v>
+      </c>
+      <c r="J20">
+        <v>3.2</v>
+      </c>
+      <c r="K20">
+        <v>1.6E-2</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12">
+      <c r="C21">
+        <v>0.82240999999999997</v>
+      </c>
+      <c r="D21">
+        <v>0.17759</v>
+      </c>
+      <c r="E21">
+        <v>133.72999999999999</v>
+      </c>
+      <c r="F21">
+        <v>120.31</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>3.4</v>
+      </c>
+      <c r="J21">
+        <v>3.4</v>
+      </c>
+      <c r="K21">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12">
+      <c r="C22">
+        <v>0.84157999999999999</v>
+      </c>
+      <c r="D22">
+        <v>0.15842000000000001</v>
+      </c>
+      <c r="E22">
+        <v>130.46</v>
+      </c>
+      <c r="F22">
+        <v>116.8</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>3.6</v>
+      </c>
+      <c r="J22">
+        <v>3.6</v>
+      </c>
+      <c r="K22">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12">
+      <c r="C23">
+        <v>0.8579</v>
+      </c>
+      <c r="D23">
+        <v>0.1421</v>
+      </c>
+      <c r="E23">
+        <v>127.12</v>
+      </c>
+      <c r="F23">
+        <v>113.23</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>3.8</v>
+      </c>
+      <c r="J23">
+        <v>3.8</v>
+      </c>
+      <c r="K23">
+        <v>1.9E-2</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12">
+      <c r="C24">
+        <v>0.87160000000000004</v>
+      </c>
+      <c r="D24">
+        <v>0.12839999999999999</v>
+      </c>
+      <c r="E24">
+        <v>123.71</v>
+      </c>
+      <c r="F24">
+        <v>109.62</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>4.0000999999999998</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <v>0.02</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12">
+      <c r="C25">
+        <v>0.88292999999999999</v>
+      </c>
+      <c r="D25">
+        <v>0.11706999999999999</v>
+      </c>
+      <c r="E25">
+        <v>120.26</v>
+      </c>
+      <c r="F25">
+        <v>105.98</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>4.2000999999999999</v>
+      </c>
+      <c r="J25">
+        <v>4.2</v>
+      </c>
+      <c r="K25">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12">
+      <c r="C26">
+        <v>0.89212000000000002</v>
+      </c>
+      <c r="D26">
+        <v>0.10788</v>
+      </c>
+      <c r="E26">
+        <v>116.76</v>
+      </c>
+      <c r="F26">
+        <v>102.32</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>4.4001000000000001</v>
+      </c>
+      <c r="J26">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12">
+      <c r="C27">
+        <v>0.89939999999999998</v>
+      </c>
+      <c r="D27">
+        <v>0.10059999999999999</v>
+      </c>
+      <c r="E27">
+        <v>113.23</v>
+      </c>
+      <c r="F27">
+        <v>98.644000000000005</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>4.6001000000000003</v>
+      </c>
+      <c r="J27">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K27">
+        <v>2.3E-2</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12">
+      <c r="C28">
+        <v>0.90500999999999998</v>
+      </c>
+      <c r="D28">
+        <v>9.4987000000000002E-2</v>
+      </c>
+      <c r="E28">
+        <v>109.66</v>
+      </c>
+      <c r="F28">
+        <v>94.962999999999994</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>4.8000999999999996</v>
+      </c>
+      <c r="J28">
+        <v>4.8</v>
+      </c>
+      <c r="K28">
+        <v>2.4E-2</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12">
+      <c r="C29">
+        <v>0.90922000000000003</v>
+      </c>
+      <c r="D29">
+        <v>9.0777999999999998E-2</v>
+      </c>
+      <c r="E29">
+        <v>106.07</v>
+      </c>
+      <c r="F29">
+        <v>91.283000000000001</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>5.0000999999999998</v>
+      </c>
+      <c r="J29">
+        <v>5</v>
+      </c>
+      <c r="K29">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12">
+      <c r="C30">
+        <v>0.91227000000000003</v>
+      </c>
+      <c r="D30">
+        <v>8.7725999999999998E-2</v>
+      </c>
+      <c r="E30">
+        <v>102.47</v>
+      </c>
+      <c r="F30">
+        <v>87.608000000000004</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>5.2000999999999999</v>
+      </c>
+      <c r="J30">
+        <v>5.2</v>
+      </c>
+      <c r="K30">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12">
+      <c r="C31">
+        <v>0.91440999999999995</v>
+      </c>
+      <c r="D31">
+        <v>8.5586999999999996E-2</v>
+      </c>
+      <c r="E31">
+        <v>98.846999999999994</v>
+      </c>
+      <c r="F31">
+        <v>83.936999999999998</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>5.4001000000000001</v>
+      </c>
+      <c r="J31">
+        <v>5.4</v>
+      </c>
+      <c r="K31">
+        <v>2.7E-2</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12">
+      <c r="C32">
+        <v>0.91586000000000001</v>
+      </c>
+      <c r="D32">
+        <v>8.4140999999999994E-2</v>
+      </c>
+      <c r="E32">
+        <v>95.216999999999999</v>
+      </c>
+      <c r="F32">
+        <v>80.272999999999996</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>5.6001000000000003</v>
+      </c>
+      <c r="J32">
+        <v>5.6</v>
+      </c>
+      <c r="K32">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12">
+      <c r="C33">
+        <v>0.91679999999999995</v>
+      </c>
+      <c r="D33">
+        <v>8.3200999999999997E-2</v>
+      </c>
+      <c r="E33">
+        <v>91.58</v>
+      </c>
+      <c r="F33">
+        <v>76.614000000000004</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>5.8000999999999996</v>
+      </c>
+      <c r="J33">
+        <v>5.8</v>
+      </c>
+      <c r="K33">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12">
+      <c r="C34">
+        <v>0.91739000000000004</v>
+      </c>
+      <c r="D34">
+        <v>8.2612000000000005E-2</v>
+      </c>
+      <c r="E34">
+        <v>87.938999999999993</v>
+      </c>
+      <c r="F34">
+        <v>72.959000000000003</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>6.0000999999999998</v>
+      </c>
+      <c r="J34">
+        <v>6</v>
+      </c>
+      <c r="K34">
+        <v>0.03</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12">
+      <c r="C35">
+        <v>0.91774</v>
+      </c>
+      <c r="D35">
+        <v>8.2256999999999997E-2</v>
+      </c>
+      <c r="E35">
+        <v>84.296000000000006</v>
+      </c>
+      <c r="F35">
+        <v>69.307000000000002</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>6.2000999999999999</v>
+      </c>
+      <c r="J35">
+        <v>6.2</v>
+      </c>
+      <c r="K35">
+        <v>3.1E-2</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12">
+      <c r="C36">
+        <v>0.91795000000000004</v>
+      </c>
+      <c r="D36">
+        <v>8.2049999999999998E-2</v>
+      </c>
+      <c r="E36">
+        <v>80.650000000000006</v>
+      </c>
+      <c r="F36">
+        <v>65.656000000000006</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>6.4001000000000001</v>
+      </c>
+      <c r="J36">
+        <v>6.4</v>
+      </c>
+      <c r="K36">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12">
+      <c r="C37">
+        <v>0.91805999999999999</v>
+      </c>
+      <c r="D37">
+        <v>8.1934999999999994E-2</v>
+      </c>
+      <c r="E37">
+        <v>77.004000000000005</v>
+      </c>
+      <c r="F37">
+        <v>62.006999999999998</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>6.6001000000000003</v>
+      </c>
+      <c r="J37">
+        <v>6.6</v>
+      </c>
+      <c r="K37">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12">
+      <c r="C38">
+        <v>0.91813</v>
+      </c>
+      <c r="D38">
+        <v>8.1873000000000001E-2</v>
+      </c>
+      <c r="E38">
+        <v>73.356999999999999</v>
+      </c>
+      <c r="F38">
+        <v>58.359000000000002</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>6.8000999999999996</v>
+      </c>
+      <c r="J38">
+        <v>6.8</v>
+      </c>
+      <c r="K38">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12">
+      <c r="C39">
+        <v>0.91815999999999998</v>
+      </c>
+      <c r="D39">
+        <v>8.1840999999999997E-2</v>
+      </c>
+      <c r="E39">
+        <v>69.709999999999994</v>
+      </c>
+      <c r="F39">
+        <v>54.710999999999999</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>7.0000999999999998</v>
+      </c>
+      <c r="J39">
+        <v>7</v>
+      </c>
+      <c r="K39">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12">
+      <c r="C40">
+        <v>0.91818</v>
+      </c>
+      <c r="D40">
+        <v>8.1823999999999994E-2</v>
+      </c>
+      <c r="E40">
+        <v>66.063000000000002</v>
+      </c>
+      <c r="F40">
+        <v>51.064</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>7.2000999999999999</v>
+      </c>
+      <c r="J40">
+        <v>7.2</v>
+      </c>
+      <c r="K40">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12">
+      <c r="C41">
+        <v>0.91818</v>
+      </c>
+      <c r="D41">
+        <v>8.1817000000000001E-2</v>
+      </c>
+      <c r="E41">
+        <v>62.415999999999997</v>
+      </c>
+      <c r="F41">
+        <v>47.415999999999997</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>7.4001000000000001</v>
+      </c>
+      <c r="J41">
+        <v>7.4</v>
+      </c>
+      <c r="K41">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12">
+      <c r="C42">
+        <v>0.91818999999999995</v>
+      </c>
+      <c r="D42">
+        <v>8.1812999999999997E-2</v>
+      </c>
+      <c r="E42">
+        <v>58.768999999999998</v>
+      </c>
+      <c r="F42">
+        <v>43.768999999999998</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>7.6001000000000003</v>
+      </c>
+      <c r="J42">
+        <v>7.6</v>
+      </c>
+      <c r="K42">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12">
+      <c r="C43">
+        <v>0.91818999999999995</v>
+      </c>
+      <c r="D43">
+        <v>8.1810999999999995E-2</v>
+      </c>
+      <c r="E43">
+        <v>55.121000000000002</v>
+      </c>
+      <c r="F43">
+        <v>40.121000000000002</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>7.8000999999999996</v>
+      </c>
+      <c r="J43">
+        <v>7.8</v>
+      </c>
+      <c r="K43">
+        <v>3.9E-2</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12">
+      <c r="C44">
+        <v>0.91818999999999995</v>
+      </c>
+      <c r="D44">
+        <v>8.1809999999999994E-2</v>
+      </c>
+      <c r="E44">
+        <v>51.473999999999997</v>
+      </c>
+      <c r="F44">
+        <v>36.473999999999997</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>8.0000999999999998</v>
+      </c>
+      <c r="J44">
+        <v>8</v>
+      </c>
+      <c r="K44">
+        <v>0.04</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12">
+      <c r="C45">
+        <v>0.91818999999999995</v>
+      </c>
+      <c r="D45">
+        <v>8.1809999999999994E-2</v>
+      </c>
+      <c r="E45">
+        <v>47.826000000000001</v>
+      </c>
+      <c r="F45">
+        <v>32.826000000000001</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>8.2001000000000008</v>
+      </c>
+      <c r="J45">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K45">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12">
+      <c r="C46">
+        <v>0.91818999999999995</v>
+      </c>
+      <c r="D46">
+        <v>8.1809999999999994E-2</v>
+      </c>
+      <c r="E46">
+        <v>44.179000000000002</v>
+      </c>
+      <c r="F46">
+        <v>29.178999999999998</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>8.4001000000000001</v>
+      </c>
+      <c r="J46">
+        <v>8.4</v>
+      </c>
+      <c r="K46">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12">
+      <c r="C47">
+        <v>0.91818999999999995</v>
+      </c>
+      <c r="D47">
+        <v>8.1809999999999994E-2</v>
+      </c>
+      <c r="E47">
+        <v>40.531999999999996</v>
+      </c>
+      <c r="F47">
+        <v>25.532</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>8.6000999999999994</v>
+      </c>
+      <c r="J47">
+        <v>8.6</v>
+      </c>
+      <c r="K47">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12">
+      <c r="C48">
+        <v>0.91818999999999995</v>
+      </c>
+      <c r="D48">
+        <v>8.1809999999999994E-2</v>
+      </c>
+      <c r="E48">
+        <v>36.884</v>
+      </c>
+      <c r="F48">
+        <v>21.884</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>8.8001000000000005</v>
+      </c>
+      <c r="J48">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="K48">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12">
+      <c r="C49">
+        <v>0.91818999999999995</v>
+      </c>
+      <c r="D49">
+        <v>8.1809999999999994E-2</v>
+      </c>
+      <c r="E49">
+        <v>33.237000000000002</v>
+      </c>
+      <c r="F49">
+        <v>18.236999999999998</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>9.0000999999999998</v>
+      </c>
+      <c r="J49">
+        <v>9</v>
+      </c>
+      <c r="K49">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12">
+      <c r="C50">
+        <v>0.91818999999999995</v>
+      </c>
+      <c r="D50">
+        <v>8.1809999999999994E-2</v>
+      </c>
+      <c r="E50">
+        <v>29.59</v>
+      </c>
+      <c r="F50">
+        <v>14.59</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>9.2001000000000008</v>
+      </c>
+      <c r="J50">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="K50">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12">
+      <c r="C51">
+        <v>0.91818999999999995</v>
+      </c>
+      <c r="D51">
+        <v>8.1809999999999994E-2</v>
+      </c>
+      <c r="E51">
+        <v>25.942</v>
+      </c>
+      <c r="F51">
+        <v>10.942</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>9.4001000000000001</v>
+      </c>
+      <c r="J51">
+        <v>9.4</v>
+      </c>
+      <c r="K51">
+        <v>4.7E-2</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="3:12">
+      <c r="C52">
+        <v>0.91818999999999995</v>
+      </c>
+      <c r="D52">
+        <v>8.1809999999999994E-2</v>
+      </c>
+      <c r="E52">
+        <v>22.295000000000002</v>
+      </c>
+      <c r="F52">
+        <v>7.2948000000000004</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>9.6000999999999994</v>
+      </c>
+      <c r="J52">
+        <v>9.6</v>
+      </c>
+      <c r="K52">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="3:12">
+      <c r="C53">
+        <v>0.91818999999999995</v>
+      </c>
+      <c r="D53">
+        <v>8.1809999999999994E-2</v>
+      </c>
+      <c r="E53">
+        <v>18.646999999999998</v>
+      </c>
+      <c r="F53">
+        <v>3.6474000000000002</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>9.8001000000000005</v>
+      </c>
+      <c r="J53">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="K53">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="3:12">
+      <c r="C54">
+        <v>0.91818999999999995</v>
+      </c>
+      <c r="D54">
+        <v>8.1809999999999994E-2</v>
+      </c>
+      <c r="E54">
+        <v>15</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>10</v>
+      </c>
+      <c r="J54">
+        <v>10</v>
+      </c>
+      <c r="K54">
+        <v>0.05</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C3:L54"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
@@ -4858,7 +6568,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:D33"/>
   <sheetViews>

</xml_diff>